<commit_message>
After 3x 1e5 MC runs for cross validation
</commit_message>
<xml_diff>
--- a/Figures/Tables/MIMICS_HiRes_pub_tables.xlsx
+++ b/Figures/Tables/MIMICS_HiRes_pub_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\MIMICS_HiRes\Figures\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82B8084-C15F-4997-8A70-B19769E08782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DF894D-8EBC-48CA-8CAF-116627F02F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="624" windowWidth="30240" windowHeight="12708" xr2:uid="{5F00AD6A-5158-4D83-ADD0-032A6CA63057}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{5F00AD6A-5158-4D83-ADD0-032A6CA63057}"/>
   </bookViews>
   <sheets>
     <sheet name="MIMICS Parms Redux" sheetId="3" r:id="rId1"/>
@@ -1054,30 +1054,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Table 1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>MIMICS parameters included in the Monte Carlo Markov Chain (MCMC) determination and the best-fit values found for the Reynolds Creek Experimental Watershed and Critical Zone Observatory (RCEW-CZO) calibration data.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">0.4 </t>
     </r>
     <r>
@@ -1106,15 +1082,9 @@
     <t>0.4 – 4</t>
   </si>
   <si>
-    <t>0.5 – 1.5</t>
-  </si>
-  <si>
     <t>0.001 – 0.3</t>
   </si>
   <si>
-    <t>0.3 – 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">   deviation is derived from the parameter ensemble (n=30) with RMSE 1.8-2.0.   </t>
   </si>
   <si>
@@ -1134,6 +1104,197 @@
   </si>
   <si>
     <r>
+      <t>Best-Fit Scaling Factor</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+  </si>
+  <si>
+    <t>0.017, 0.027, 0.017</t>
+  </si>
+  <si>
+    <r>
+      <t>0.30 × e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1.3(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>clay)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 0.20 × e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0.8(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">clay) </t>
+    </r>
+  </si>
+  <si>
+    <t>0.55, 0.25, 0.75, 0.35</t>
+  </si>
+  <si>
+    <r>
+      <t>0.015 × e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1.3(fclay)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 0.01 × e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0.8(fclay)</t>
+    </r>
+  </si>
+  <si>
+    <t>Desorption rate from SOMp to SOMa</t>
+  </si>
+  <si>
+    <r>
+      <t>Scaling Factor Proposal Range</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  See Methods for further details.</t>
+  </si>
+  <si>
+    <t>0.01 – 4</t>
+  </si>
+  <si>
+    <t>0.2 – 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>MIMICS parameters included in the Monte Carlo (MC) optimization determination and the best-fit values found for the Reynolds Creek Experimental Watershed and Critical Zone Observatory (RCEW-CZO) calibration data.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <vertAlign val="superscript"/>
         <sz val="10"/>
@@ -1150,13 +1311,10 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> Further information regarding MIMICS parameters and default values provided in Wieder et al. 2015.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Best-Fit Scaling Factor</t>
-    </r>
+      <t xml:space="preserve"> Further information regarding MIMICS parameters and default initial values provided in Wieder et al. 2015.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
@@ -1174,153 +1332,10 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">            </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Parameter proposals in the MCMC algorithm were conveyed as a factor of the initial prior value(s). Presented standard </t>
-    </r>
-  </si>
-  <si>
-    <t>0.017, 0.027, 0.017</t>
-  </si>
-  <si>
-    <r>
-      <t>0.30 × e</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1.3(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>clay)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, 0.20 × e</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>0.8(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">clay) </t>
-    </r>
-  </si>
-  <si>
-    <t>0.55, 0.25, 0.75, 0.35</t>
-  </si>
-  <si>
-    <r>
-      <t>0.015 × e</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1.3(fclay)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, 0.01 × e</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>0.8(fclay)</t>
-    </r>
-  </si>
-  <si>
-    <t>Desorption rate from SOMp to SOMa</t>
-  </si>
-  <si>
-    <r>
-      <t>Scaling Factor Proposal Range</t>
-    </r>
+      <t xml:space="preserve"> Parameter proposals in the MC algorithm were conveyed as a factor of the initial prior value(s). Presented standard </t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
@@ -1331,30 +1346,15 @@
       </rPr>
       <t>c</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Factor proposals for each parameter were confined to agree with natural analogs and reduce computational demands. </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">  See Methods for further details.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Factor proposals for each parameter were confined to agree with natural analogs and to reduce computational demands. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1437,7 +1437,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1447,6 +1447,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1483,7 +1489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1575,13 +1581,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1602,72 +1614,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDE4729A-F5E4-428B-95E5-3EBA8E75FDFD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9096375" y="457200"/>
-          <a:ext cx="6172200" cy="5153025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1970,36 +1916,36 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="7.5546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="11" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2007,13 +1953,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>71</v>
+        <v>59</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>2</v>
@@ -2023,7 +1969,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>14</v>
       </c>
@@ -2037,7 +1983,7 @@
         <v>46</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>15</v>
@@ -2047,7 +1993,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
@@ -2061,7 +2007,7 @@
         <v>47</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>17</v>
@@ -2071,7 +2017,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
@@ -2079,13 +2025,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>48</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>19</v>
@@ -2095,7 +2041,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>20</v>
       </c>
@@ -2109,7 +2055,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>21</v>
@@ -2119,7 +2065,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>3</v>
       </c>
@@ -2127,13 +2073,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>50</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>23</v>
@@ -2143,7 +2089,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>7</v>
       </c>
@@ -2151,13 +2097,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>22</v>
@@ -2167,12 +2113,12 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>45</v>
@@ -2181,7 +2127,7 @@
         <v>52</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>23</v>
@@ -2191,7 +2137,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>24</v>
       </c>
@@ -2199,13 +2145,13 @@
         <v>12</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>53</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>13</v>
@@ -2215,9 +2161,9 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2229,9 +2175,9 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -2243,9 +2189,9 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
@@ -2257,9 +2203,9 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
-        <v>72</v>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>73</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -2271,9 +2217,9 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>73</v>
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>67</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2285,7 +2231,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2297,7 +2243,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -2309,7 +2255,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -2321,7 +2267,7 @@
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -2333,7 +2279,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -2345,7 +2291,7 @@
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -2357,7 +2303,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2369,7 +2315,7 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2381,7 +2327,7 @@
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2393,7 +2339,7 @@
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -2405,7 +2351,7 @@
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -2417,7 +2363,7 @@
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2429,7 +2375,7 @@
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -2441,7 +2387,7 @@
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -2459,7 +2405,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2471,31 +2416,31 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="9.5546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2516,7 +2461,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -2537,7 +2482,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -2558,7 +2503,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -2579,7 +2524,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -2600,7 +2545,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -2621,7 +2566,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -2642,7 +2587,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -2663,7 +2608,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
@@ -2684,7 +2629,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
@@ -2697,7 +2642,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -2710,7 +2655,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -2723,7 +2668,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -2736,7 +2681,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -2749,7 +2694,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -2760,7 +2705,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -2771,7 +2716,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -2782,7 +2727,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -2793,7 +2738,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -2804,7 +2749,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -2815,7 +2760,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2826,7 +2771,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2837,7 +2782,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2848,7 +2793,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -2859,7 +2804,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -2870,7 +2815,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2881,7 +2826,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -2892,7 +2837,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>

</xml_diff>